<commit_message>
change short description of boiteLettreMSS 4d1a65412c232e1eb4922be02c6790868ab56e92
</commit_message>
<xml_diff>
--- a/sg/ressources-changes-v43/ig/StructureDefinition-ror-organization.xlsx
+++ b/sg/ressources-changes-v43/ig/StructureDefinition-ror-organization.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-02T14:19:26+00:00</t>
+    <t>2025-10-02T15:49:09+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1839,7 +1839,7 @@
 </t>
   </si>
   <si>
-    <t>boiteLettreMSS (OffreOperationnelle) : Boîte(s) aux lettres du service de messagerie sécurisée de santé (MSS) rattachée(s) à l’organisation interne</t>
+    <t>boiteLettreMSS (OrganisationInterne) : Boîte(s) aux lettres du service de messagerie sécurisée de santé (MSS) rattachée(s) à l’organisation interne</t>
   </si>
   <si>
     <t>Details for all kinds of technology mediated contact points for a person or organization, including telephone, email, etc.</t>

</xml_diff>